<commit_message>
submit recording and vods
</commit_message>
<xml_diff>
--- a/testCase/casedata/recordingVods_casedata.xlsx
+++ b/testCase/casedata/recordingVods_casedata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>base_url</t>
   </si>
@@ -59,6 +59,24 @@
   </si>
   <si>
     <t>https://sdk.xylink.com/api/rest/external/v1/vods/</t>
+  </si>
+  <si>
+    <t>get_sharedInfo_accordVodId</t>
+  </si>
+  <si>
+    <t>get_getdownloadurl_accordVodId</t>
+  </si>
+  <si>
+    <t>delete_vod_accordMeetingRoomNumber</t>
+  </si>
+  <si>
+    <t>get_vodsList_accordMeetingId</t>
+  </si>
+  <si>
+    <t>get_thumbnailurl_accordVodId</t>
+  </si>
+  <si>
+    <t>query_vodsList_accordLiveId</t>
   </si>
 </sst>
 </file>
@@ -96,7 +114,60 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -110,30 +181,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,14 +205,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,29 +226,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -202,23 +236,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,187 +251,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,56 +442,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -505,7 +473,37 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,6 +522,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -532,10 +550,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -544,16 +562,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -562,115 +580,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1000,13 +1018,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="35.375" customWidth="1"/>
     <col min="2" max="2" width="67.125" customWidth="1"/>
@@ -1070,6 +1088,54 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1082,6 +1148,12 @@
     <hyperlink ref="B6" r:id="rId5" display="https://sdk.xylink.com/api/rest/external/v1/nemo/"/>
     <hyperlink ref="B7" r:id="rId6" display="https://sdk.xylink.com/api/rest/external/v1/vods/page"/>
     <hyperlink ref="B8" r:id="rId7" display="https://sdk.xylink.com/api/rest/external/v1/vods/"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://sdk.xylink.com/api/rest/external/v1/vods/"/>
+    <hyperlink ref="B10" r:id="rId7" display="https://sdk.xylink.com/api/rest/external/v1/vods/"/>
+    <hyperlink ref="B11" r:id="rId4" display="https://sdk.xylink.com/api/rest/external/v1/meetingroom/"/>
+    <hyperlink ref="B12" r:id="rId4" display="https://sdk.xylink.com/api/rest/external/v1/meetingroom/"/>
+    <hyperlink ref="B13" r:id="rId7" display="https://sdk.xylink.com/api/rest/external/v1/vods/"/>
+    <hyperlink ref="B14" r:id="rId7" display="https://sdk.xylink.com/api/rest/external/v1/vods/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add recording and stoprecording case
</commit_message>
<xml_diff>
--- a/testCase/casedata/recordingVods_casedata.xlsx
+++ b/testCase/casedata/recordingVods_casedata.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7860"/>
+    <workbookView windowWidth="20490" windowHeight="7860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="base_url" sheetId="1" r:id="rId1"/>
+    <sheet name="test_data" sheetId="2" r:id="rId2"/>
+    <sheet name="ExpectedResult" sheetId="3" r:id="rId3"/>
+    <sheet name="responseData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>base_url</t>
   </si>
@@ -59,6 +62,18 @@
   </si>
   <si>
     <t>https://sdk.xylink.com/api/rest/external/v1/vods/</t>
+  </si>
+  <si>
+    <t>test_StartRecording001</t>
+  </si>
+  <si>
+    <t>meetingRoomNumber:9005853980</t>
+  </si>
+  <si>
+    <t>test_StopRecording001</t>
+  </si>
+  <si>
+    <t>expected_code:200</t>
   </si>
 </sst>
 </file>
@@ -89,6 +104,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -97,6 +120,97 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -112,35 +226,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -148,77 +233,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,187 +248,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,34 +444,19 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -473,15 +473,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,6 +515,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -532,10 +547,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -544,16 +559,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -562,121 +577,124 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
@@ -1002,8 +1020,8 @@
   <sheetPr/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -1021,7 +1039,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1029,7 +1047,7 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1037,7 +1055,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1045,7 +1063,7 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1053,7 +1071,7 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1061,7 +1079,7 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1069,7 +1087,7 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1086,4 +1104,94 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="32.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="24.375" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>